<commit_message>
Added the option to choose a starting date.
refactor(dashboard): streamline data initialization and impedance analysis

Refactored the dashboard components to remove redundant DataFrame initialization and streamline impedance analysis. The changes include:
- Removing redundant DataFrame initialization in tab components by using `wound_data_processor.df`
- Updating impedance measurement field names for consistency
- Simplifying the initialization of `WoundDataProcessor` and `ImpedanceAnalyzer`
- Adding logging for better debugging and traceability
</commit_message>
<xml_diff>
--- a/dataset/impedance_frequency_sweep/41.xlsx
+++ b/dataset/impedance_frequency_sweep/41.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\GitHubs\postdoc\wound_EHR_analyzer_private\dataset\impedance_frequency_sweep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EE8C61-7D42-4E69-A31D-A6B15269036C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2290D9-69C9-426D-A2D2-29388E3F5CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="27196" windowHeight="16366" firstSheet="5" activeTab="7" xr2:uid="{F3E518EB-D0E8-49D9-8819-1E93F8F08176}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27196" windowHeight="15781" xr2:uid="{F3E518EB-D0E8-49D9-8819-1E93F8F08176}"/>
   </bookViews>
   <sheets>
     <sheet name="Impedance Spectroscopy 1 S11" sheetId="12" r:id="rId1"/>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9D0611-C327-4F6E-8488-AAB71E1EC4F5}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5090,7 +5090,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E83CA8F9-215D-4E90-8434-94D03958913C}">
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="A2:G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -7483,7 +7485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E713B55-5FAB-4610-BD5E-1C206B43B5E6}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -10522,7 +10524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9028A2A-A742-49E6-B936-D435DC3B83A1}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>